<commit_message>
Chile File transfer developed
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolishSpain\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolisChile\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57DF65A-2228-4C9F-B87B-E5A26361CA35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769416F0-2CD8-4D59-ABDE-5152F3B68A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -150,15 +150,6 @@
     <t>DirectirioSheetName</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS 2021/33 Envio Semana 31/ESPAÑA/BD Consolidada</t>
-  </si>
-  <si>
-    <t>REPORTE_ESTUDIOC_ESPANIA_46</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/33 Envio Semana 31/ESPAÑA/BD Consolidada/Exportada</t>
-  </si>
-  <si>
     <t>DirectorioFilePath</t>
   </si>
   <si>
@@ -175,6 +166,24 @@
   </si>
   <si>
     <t>/Planeacion/0.Envios TS 2021/33 Envio Semana 31/ESPAÑA/LUXURY</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/32 Envio Semana 32</t>
+  </si>
+  <si>
+    <t>REPORTE_ESTUDIOC_CHILE_SEM_49</t>
+  </si>
+  <si>
+    <t>SurveyATMSheetName</t>
+  </si>
+  <si>
+    <t>SurveyATMFilePath</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/32 Envio Semana 32/CHILE/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/32 Envio Semana 32/CHILE/Base de Datos/Exportadas</t>
   </si>
 </sst>
 </file>
@@ -676,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -704,7 +713,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -715,7 +724,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75">
@@ -743,7 +752,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -756,7 +765,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B9" s="22"/>
     </row>
@@ -765,7 +774,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -781,7 +790,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -797,7 +806,7 @@
         <v>35</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -813,7 +822,7 @@
         <v>37</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -827,14 +836,20 @@
     <row r="21" spans="1:2">
       <c r="A21" s="2"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="15.75">
       <c r="A22" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -842,55 +857,68 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="16">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B29" s="19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="2" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B30" s="20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="4" t="s">
+    <row r="31" spans="1:2">
+      <c r="A31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B31" s="20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75">
-      <c r="A30" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="21" t="s">
+    <row r="33" spans="1:2" ht="15.75">
+      <c r="A33" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75">
-      <c r="A31" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>47</v>
+    <row r="34" spans="1:2" ht="15.75">
+      <c r="A34" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B26" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
+    <hyperlink ref="B29" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
chile run updated for this week only
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolisChile\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769416F0-2CD8-4D59-ABDE-5152F3B68A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53FADE2-FAC3-4946-BC3B-5671EF56E664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -184,13 +184,62 @@
   </si>
   <si>
     <t>/Planeacion/0.Envios TS 2021/32 Envio Semana 32/CHILE/Base de Datos/Exportadas</t>
+  </si>
+  <si>
+    <t>CHILE</t>
+  </si>
+  <si>
+    <t>/Planning/0.Shipping TS 2021/1 Directory</t>
+  </si>
+  <si>
+    <t>DataNoBelongToCurrentWeekMailSubject</t>
+  </si>
+  <si>
+    <t>Notification- Data doesn't belong to this week</t>
+  </si>
+  <si>
+    <t>DataNoBelongToCurrentWeekMailBody</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+Please find the below data which does not belong to current week.&lt;br/&gt;
+[Nothisweekdatatable]
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>MailTo</t>
+  </si>
+  <si>
+    <t>MailCC</t>
+  </si>
+  <si>
+    <t>manindersinghbisht77@gmail.com</t>
+  </si>
+  <si>
+    <t>InputFileExceptionSubject</t>
+  </si>
+  <si>
+    <t>Error- Input file Notification</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+There is a error in Cline run, below is the detail of error&lt;br/&gt;
+[error]
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>InputFileExceptionbody</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -312,6 +361,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -330,10 +385,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -371,8 +427,16 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -687,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -855,14 +919,20 @@
     <row r="24" spans="1:2">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" ht="15.75">
       <c r="A25" s="2" t="s">
         <v>40</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
         <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -929,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1005,18 +1075,55 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="B5" s="13"/>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B7" s="2"/>
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="B8" s="9"/>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1984,8 +2091,11 @@
     <row r="978" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{6FB6AAA5-47EC-4559-A8F8-E0E4F851D044}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
config file updated from test environment
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolisChile\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisChile\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53FADE2-FAC3-4946-BC3B-5671EF56E664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C48095-EA29-4CFF-BDD8-2B769F58AEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -99,9 +99,6 @@
     <t>input file path for non partner file</t>
   </si>
   <si>
-    <t>BD_ENCUESTA_LARGA_GULF_Tradicio</t>
-  </si>
-  <si>
     <t>BDVIPfilePath</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>SurveyVipSheetName</t>
   </si>
   <si>
-    <t>BD_ENCUESTA_LARGA_GULF_VIP_Sema</t>
-  </si>
-  <si>
     <t>DirectirioFilePath</t>
   </si>
   <si>
@@ -156,21 +150,9 @@
     <t>DirectorioSheetName</t>
   </si>
   <si>
-    <t>España</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/33 Envio Semana 31/ESPAÑA/TRADICIONAL</t>
-  </si>
-  <si>
     <t>BDTempFileName</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS 2021/33 Envio Semana 31/ESPAÑA/LUXURY</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/32 Envio Semana 32</t>
-  </si>
-  <si>
     <t>REPORTE_ESTUDIOC_CHILE_SEM_49</t>
   </si>
   <si>
@@ -180,16 +162,19 @@
     <t>SurveyATMFilePath</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS 2021/32 Envio Semana 32/CHILE/Base de Datos</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/32 Envio Semana 32/CHILE/Base de Datos/Exportadas</t>
+    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/CHILE/Base de Datos</t>
+  </si>
+  <si>
+    <t>BD_Chile_VIP_Semana_06_12_ dic</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/CHILE/TRADICIONAL</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/CHILE/Base de Datos/Exportadas</t>
   </si>
   <si>
     <t>CHILE</t>
-  </si>
-  <si>
-    <t>/Planning/0.Shipping TS 2021/1 Directory</t>
   </si>
   <si>
     <t>DataNoBelongToCurrentWeekMailSubject</t>
@@ -212,16 +197,19 @@
     <t>MailTo</t>
   </si>
   <si>
+    <t>manindersinghbisht77@gmail.com</t>
+  </si>
+  <si>
     <t>MailCC</t>
   </si>
   <si>
-    <t>manindersinghbisht77@gmail.com</t>
-  </si>
-  <si>
     <t>InputFileExceptionSubject</t>
   </si>
   <si>
     <t>Error- Input file Notification</t>
+  </si>
+  <si>
+    <t>InputFileExceptionbody</t>
   </si>
   <si>
     <t>Dear Team&lt;br/&gt;
@@ -230,9 +218,6 @@
 Also let us know if anything is required&lt;br/&gt;
 Thank you,&lt;br/&gt;
 **********************This is system generated E-Mail, please do not respond on this************</t>
-  </si>
-  <si>
-    <t>InputFileExceptionbody</t>
   </si>
 </sst>
 </file>
@@ -389,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -427,12 +412,11 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -752,7 +736,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B33" sqref="B33:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -777,7 +761,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -785,26 +769,26 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75">
       <c r="A5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75">
@@ -813,40 +797,35 @@
     </row>
     <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B9" s="22"/>
     </row>
     <row r="10" spans="1:3" ht="15.75">
       <c r="A10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>45</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B10" s="21"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75">
@@ -854,7 +833,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -867,15 +846,15 @@
     </row>
     <row r="16" spans="1:3" ht="15.75">
       <c r="A16" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
@@ -883,15 +862,15 @@
     </row>
     <row r="19" spans="1:2" ht="15.75">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
@@ -902,15 +881,15 @@
     </row>
     <row r="22" spans="1:2" ht="15.75">
       <c r="A22" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
         <v>14</v>
@@ -919,20 +898,20 @@
     <row r="24" spans="1:2">
       <c r="A24" s="2"/>
     </row>
-    <row r="25" spans="1:2" ht="15.75">
+    <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>55</v>
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -972,18 +951,18 @@
     </row>
     <row r="33" spans="1:2" ht="15.75">
       <c r="A33" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75">
       <c r="A34" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -999,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1076,52 +1055,57 @@
       <c r="B5" s="13"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
+      <c r="A6" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" s="23"/>
+      <c r="B8" s="25"/>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="23" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
+      <c r="B10" s="23"/>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B8" s="9"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
+      <c r="B13" s="24" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2092,7 +2076,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{6FB6AAA5-47EC-4559-A8F8-E0E4F851D044}"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{FADAD646-DE63-45C2-8209-E28F2445EE90}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
correct name implimented in chile
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisChile\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A20B32B-C2EC-4FFF-833B-7181E52824D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E57B6B-5AB1-4D20-9D11-BDB2C7BECA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>BaseTrackingChile10al16Enero</t>
+  </si>
+  <si>
+    <t>CorrectnameFilePath</t>
+  </si>
+  <si>
+    <t>CorrectSheetName</t>
   </si>
 </sst>
 </file>
@@ -733,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -963,6 +969,16 @@
       </c>
       <c r="B34" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -979,7 +995,7 @@
   <dimension ref="A1:Z978"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
chile is updated and tested
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisChile\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E57B6B-5AB1-4D20-9D11-BDB2C7BECA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B830095-5823-4035-835D-C46182D6DCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -108,18 +108,6 @@
     <t>InputSheetName</t>
   </si>
   <si>
-    <t>InputSheetNewName</t>
-  </si>
-  <si>
-    <t>InputVIPSheetName</t>
-  </si>
-  <si>
-    <t>LUXURY</t>
-  </si>
-  <si>
-    <t>TRADICIONAL</t>
-  </si>
-  <si>
     <t>BDTempFilePath</t>
   </si>
   <si>
@@ -150,24 +138,12 @@
     <t>DirectorioSheetName</t>
   </si>
   <si>
-    <t>BDTempFileName</t>
-  </si>
-  <si>
     <t>SurveyATMSheetName</t>
   </si>
   <si>
     <t>SurveyATMFilePath</t>
   </si>
   <si>
-    <t>BD_Chile_VIP_Semana_06_12_ dic</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/CHILE/TRADICIONAL</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/36 Envio Semana 36/CHILE/Base de Datos/Exportadas</t>
-  </si>
-  <si>
     <t>CHILE</t>
   </si>
   <si>
@@ -183,9 +159,6 @@
     <t>MailTo</t>
   </si>
   <si>
-    <t>manindersinghbisht77@gmail.com</t>
-  </si>
-  <si>
     <t>MailCC</t>
   </si>
   <si>
@@ -196,41 +169,138 @@
   </si>
   <si>
     <t>InputFileExceptionbody</t>
+  </si>
+  <si>
+    <t>CorrectnameFilePath</t>
+  </si>
+  <si>
+    <t>CorrectSheetName</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/CHILE/Base de Datos</t>
+  </si>
+  <si>
+    <t>REPORTE_ESTUDIOC_CHILE_SEM_06_2</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/CHILE/VIP</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/CHILE/TRADICIONAL</t>
+  </si>
+  <si>
+    <t>traditional</t>
+  </si>
+  <si>
+    <t>BDATMFilePath</t>
+  </si>
+  <si>
+    <t>BDATMSheetName</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/CHILE/ATM</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/CHILE/Base de Datos/Exportadas</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/1 Directorio/Correcciones</t>
+  </si>
+  <si>
+    <t>Hoja</t>
   </si>
   <si>
     <t>Dear Team&lt;br/&gt;
 Please find the below data which does not belong to current week.&lt;br/&gt;
-[Nothisweekdatatable]&lt;br/&gt;
+[Nothisweekdatatable]&lt;br&gt;
 Also let us know if anything is required&lt;br/&gt;
 Thank you,&lt;br/&gt;
 **********************This is system generated E-Mail, please do not respond on this************</t>
   </si>
   <si>
+    <t>rhernandez@tecnoyar.com.mx</t>
+  </si>
+  <si>
+    <t>arerodriguez@tecnoyar.com</t>
+  </si>
+  <si>
     <t>Dear Team&lt;br/&gt;
-There is a error in Cline run, below is the detail of error&lt;br/&gt;
-[error]&lt;/br&gt;
+There is a error in Cinepolish maxico run, below is the detail of error&lt;br/&gt;
+[error]&lt;br/&gt;
 Also let us know if anything is required&lt;br/&gt;
 Thank you,&lt;br/&gt;
 **********************This is system generated E-Mail, please do not respond on this************</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS 2021/2022/03 Envio Semana 03/CHILE/Base de Datos</t>
-  </si>
-  <si>
-    <t>BaseTrackingChile10al16Enero</t>
-  </si>
-  <si>
-    <t>CorrectnameFilePath</t>
-  </si>
-  <si>
-    <t>CorrectSheetName</t>
+    <t>downloadFileExceptionSubject</t>
+  </si>
+  <si>
+    <t>Notification- Not All file Got downloaded</t>
+  </si>
+  <si>
+    <t>downloadFileExceptionbody</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+There is a error in Cinepos Maxico process run, below is the detail of error&lt;br/&gt;
+Not all required files got downloaded from FTP&lt;br/&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>WrongNameMailSubject</t>
+  </si>
+  <si>
+    <t>Notification- name is not correct</t>
+  </si>
+  <si>
+    <t>WrongNameMailbody</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+below names are not correct in Maxico process input file.&lt;br/&gt;
+[wrongnamedatatable]&lt;br&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>NADirectrioMailSubject</t>
+  </si>
+  <si>
+    <t>file of the Maxico mark contains errors in the "N" column called "clave_tipo_cine"</t>
+  </si>
+  <si>
+    <t>NADirectrioMailBody</t>
+  </si>
+  <si>
+    <t>#NA data found at input file in "N" column</t>
+  </si>
+  <si>
+    <t>WorkingStartDate</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>WorkingEndDate</t>
+  </si>
+  <si>
+    <t>Key words in filename</t>
+  </si>
+  <si>
+    <t>REPORTE,ESTUDIO</t>
+  </si>
+  <si>
+    <t>Black List</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -324,12 +394,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF4E5E65"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -353,10 +417,11 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -376,17 +441,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -397,9 +458,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -414,8 +473,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -423,10 +482,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -739,251 +806,260 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="84.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75">
+      <c r="D1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>60</v>
+      <c r="B2" s="18" t="s">
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75">
-      <c r="A4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75">
+      <c r="A4" s="2"/>
+      <c r="B4" s="18"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="19"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75">
+      <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B7" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="18"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75">
+      <c r="A9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
-      <c r="A5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75">
-      <c r="A6" s="2"/>
-      <c r="B6" s="21"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.75">
-      <c r="A7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="1:3" ht="15.75">
-      <c r="A10" s="2" t="s">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75">
+      <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="21"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2" t="s">
+      <c r="B18" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="18" t="s">
+      <c r="B19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75">
-      <c r="A16" s="2" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:2" ht="15.75">
+      <c r="A21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75">
-      <c r="A19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" ht="15.75">
-      <c r="A22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="2"/>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" t="s">
-        <v>48</v>
-      </c>
+      <c r="A26" s="2"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="2"/>
+      <c r="A27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="13">
+        <v>21</v>
+      </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="16">
-        <v>21</v>
+        <v>10</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B30" s="17" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="32" spans="1:2" ht="15.75">
+      <c r="A32" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="33" spans="1:2" ht="15.75">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
         <v>40</v>
       </c>
-      <c r="B33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75">
-      <c r="A34" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" t="s">
-        <v>48</v>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>63</v>
+        <v>50</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B29" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
+    <hyperlink ref="B28" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -994,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1007,16 +1083,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1041,108 +1117,240 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="30">
-      <c r="A2" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="20">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="24" t="s">
         <v>6</v>
       </c>
+      <c r="D2" s="20"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="26" t="s">
         <v>20</v>
       </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="26" t="s">
         <v>21</v>
       </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B5" s="13"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>50</v>
-      </c>
+      <c r="A6" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>58</v>
-      </c>
+      <c r="A7" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>53</v>
-      </c>
+      <c r="A9" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="23"/>
+      <c r="A10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>56</v>
-      </c>
+      <c r="A12" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+      <c r="A13" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A18" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+    </row>
+    <row r="19" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A19" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+    </row>
+    <row r="20" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+    </row>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A21" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A22" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+    </row>
+    <row r="24" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A24" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="29">
+        <v>44599</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="20"/>
+    </row>
+    <row r="25" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A25" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="29">
+        <v>44605</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+    </row>
+    <row r="27" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+    </row>
+    <row r="28" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2091,11 +2299,8 @@
     <row r="978" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{FADAD646-DE63-45C2-8209-E28F2445EE90}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2161,17 +2366,17 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="C11" s="9"/>
+      <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="12"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="11"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2"/>
@@ -2181,22 +2386,22 @@
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B19" s="10"/>
+      <c r="B19" s="9"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B20" s="11"/>
-      <c r="C20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B21" s="14"/>
+      <c r="B21" s="12"/>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
process updated for directiro name
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisChile\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B830095-5823-4035-835D-C46182D6DCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55867499-E733-4F0E-B2E2-6BC3E0A5C8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -96,9 +96,6 @@
     <t>/Planeacion/0.Envios TS 2021/1 Directorio</t>
   </si>
   <si>
-    <t>input file path for non partner file</t>
-  </si>
-  <si>
     <t>BDVIPfilePath</t>
   </si>
   <si>
@@ -177,18 +174,6 @@
     <t>CorrectSheetName</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/CHILE/Base de Datos</t>
-  </si>
-  <si>
-    <t>REPORTE_ESTUDIOC_CHILE_SEM_06_2</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/CHILE/VIP</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/CHILE/TRADICIONAL</t>
-  </si>
-  <si>
     <t>traditional</t>
   </si>
   <si>
@@ -196,12 +181,6 @@
   </si>
   <si>
     <t>BDATMSheetName</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/CHILE/ATM</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/07 Envío Semana 07/CHILE/Base de Datos/Exportadas</t>
   </si>
   <si>
     <t>/Planeacion/0.Envios TS/1 Directorio/Correcciones</t>
@@ -294,6 +273,30 @@
   </si>
   <si>
     <t>Black List</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/CHILE/Base de Datos</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/CHILE/VIP</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/CHILE/TRADICIONAL</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/CHILE/ATM</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/09 Envío Semana 09/CHILE/Base de Datos/Exportadas</t>
+  </si>
+  <si>
+    <t>Nombre de la hoja del excel del archivo origen</t>
+  </si>
+  <si>
+    <t>Nombre del archivo origen</t>
+  </si>
+  <si>
+    <t>Reporte_Estudio_Chile 21 al 27 Febrero.csv</t>
   </si>
 </sst>
 </file>
@@ -808,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -831,7 +834,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75">
@@ -839,21 +842,24 @@
         <v>22</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
@@ -862,46 +868,46 @@
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="19"/>
     </row>
     <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="18"/>
     </row>
     <row r="9" spans="1:4" ht="15.75">
       <c r="A9" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75">
@@ -909,7 +915,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -917,20 +923,20 @@
         <v>13</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -938,15 +944,15 @@
     </row>
     <row r="18" spans="1:2" ht="15.75">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
@@ -957,15 +963,15 @@
     </row>
     <row r="21" spans="1:2" ht="15.75">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
         <v>14</v>
@@ -976,7 +982,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
@@ -984,10 +990,10 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1027,7 +1033,7 @@
     </row>
     <row r="32" spans="1:2" ht="15.75">
       <c r="A32" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
@@ -1035,26 +1041,26 @@
     </row>
     <row r="33" spans="1:2" ht="15.75">
       <c r="A33" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1070,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1156,20 +1162,20 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>42</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="20"/>
@@ -1182,20 +1188,20 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
@@ -1208,20 +1214,20 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>46</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>47</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
@@ -1234,20 +1240,20 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="20" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="20" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
@@ -1260,20 +1266,20 @@
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1">
       <c r="A18" s="20" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1">
       <c r="A19" s="20" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
@@ -1286,20 +1292,20 @@
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1">
       <c r="A21" s="25" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1">
       <c r="A22" s="25" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
@@ -1312,25 +1318,25 @@
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1">
       <c r="A24" s="20" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B24" s="29">
-        <v>44599</v>
+        <v>44613</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D24" s="20"/>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" s="20" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B25" s="29">
-        <v>44605</v>
+        <v>44619</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D25" s="20"/>
     </row>

</xml_diff>